<commit_message>
generate inner class name
</commit_message>
<xml_diff>
--- a/Test/Input/SplitTypeTest.xlsx
+++ b/Test/Input/SplitTypeTest.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\MakeConfig.Sharp\Test\Input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91BB5D8-8075-42B6-A1A3-FA40BC21D8C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25820" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="SplitTypeTest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,13 +58,41 @@
   </si>
   <si>
     <t>MyClass.Field3.Field2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MyField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MyClass.Field3.Field3.Field1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MyClass.Field3.Field3.Field2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MyClass.Field3.Field3.Field3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum{X,Y}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,61 +404,75 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.9140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="23.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -447,13 +483,25 @@
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1200001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>